<commit_message>
added new eclipse files that implements DDT, Excel, headless browse and surfire-report
</commit_message>
<xml_diff>
--- a/Data driven testing/DemoSiteDDT.xlsx
+++ b/Data driven testing/DemoSiteDDT.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="16">
   <si>
     <t>TestOne</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>true</t>
+  </si>
+  <si>
+    <t>PASS</t>
   </si>
 </sst>
 </file>
@@ -456,7 +459,7 @@
         <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -473,7 +476,7 @@
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -490,7 +493,7 @@
         <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -507,7 +510,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>